<commit_message>
env values created + upate of all tables according to new style
</commit_message>
<xml_diff>
--- a/data/ansp_employment.xlsx
+++ b/data/ansp_employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oburdash\dev\repos\standard_inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1B30C8-B2DE-4C87-9174-ACFAB3DEA640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAEEFB8-9095-40C0-97A1-F8ECE3A2F913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-43095" yWindow="2880" windowWidth="21600" windowHeight="11325" tabRatio="346" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="346" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>ATCOs in OPS</t>
   </si>
@@ -147,123 +147,9 @@
     <t>MOLDATSA</t>
   </si>
   <si>
-    <t>Albania</t>
-  </si>
-  <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
-    <t>Findland</t>
-  </si>
-  <si>
-    <t>Armenia</t>
-  </si>
-  <si>
-    <t>Austria</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Bulgaria</t>
-  </si>
-  <si>
-    <t>Croatia</t>
-  </si>
-  <si>
-    <t>Cyprus</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Turkey</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Estonia</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>Hungary</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>Latvia</t>
-  </si>
-  <si>
-    <t>Slovak Republic</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>Malta</t>
-  </si>
-  <si>
-    <t>Moldova</t>
-  </si>
-  <si>
-    <t>Maastricht</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>Denmark</t>
-  </si>
-  <si>
-    <t>Lithuania</t>
-  </si>
-  <si>
-    <t>Poland</t>
-  </si>
-  <si>
-    <t>Romania</t>
-  </si>
-  <si>
-    <t>Giorgia</t>
-  </si>
-  <si>
-    <t>Switzerland</t>
-  </si>
-  <si>
-    <t>Slovenia</t>
-  </si>
-  <si>
-    <t>Serbia Montenegro</t>
-  </si>
-  <si>
-    <t>Ukraine</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
     <t>Skeyes</t>
   </si>
   <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>North Macedonia</t>
-  </si>
-  <si>
     <t>Fintraffic ANS</t>
   </si>
   <si>
@@ -279,9 +165,6 @@
     <t>ansp</t>
   </si>
   <si>
-    <t>state</t>
-  </si>
-  <si>
     <t>Support Staff</t>
   </si>
   <si>
@@ -295,9 +178,6 @@
   </si>
   <si>
     <t>funct</t>
-  </si>
-  <si>
-    <t>All</t>
   </si>
   <si>
     <t>ECTRL Area (average)</t>
@@ -1544,13 +1424,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1566,7 +1446,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>74000</v>
@@ -1577,7 +1457,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>99000</v>
@@ -1594,695 +1474,574 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F5E44C-C8C2-4119-8BE2-279CC5806A69}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="B7" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>37</v>
+      <c r="B2" s="1">
+        <v>28517.857142857141</v>
       </c>
       <c r="C2" s="1">
-        <v>28517.857142857141</v>
+        <v>13526.717557251908</v>
       </c>
       <c r="D2" s="1">
-        <v>13526.717557251908</v>
-      </c>
-      <c r="E2" s="1">
         <v>16166.666666666668</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>38</v>
+      <c r="B3" s="1">
+        <v>134613.95348837209</v>
       </c>
       <c r="C3" s="1">
-        <v>134613.95348837209</v>
+        <v>53924.840764331209</v>
       </c>
       <c r="D3" s="1">
-        <v>53924.840764331209</v>
-      </c>
-      <c r="E3" s="1">
         <v>71273</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>40</v>
+      <c r="B4" s="1">
+        <v>23267.605633802817</v>
       </c>
       <c r="C4" s="1">
-        <v>23267.605633802817</v>
+        <v>13417.040358744394</v>
       </c>
       <c r="D4" s="1">
-        <v>13417.040358744394</v>
-      </c>
-      <c r="E4" s="1">
         <v>15795.91836734694</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>41</v>
+      <c r="B5" s="1">
+        <v>203530.90909090909</v>
       </c>
       <c r="C5" s="1">
-        <v>203530.90909090909</v>
+        <v>108389.89169675091</v>
       </c>
       <c r="D5" s="1">
-        <v>108389.89169675091</v>
-      </c>
-      <c r="E5" s="1">
         <v>139950.54282267793</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>42</v>
+      <c r="B6" s="1">
+        <v>189000</v>
       </c>
       <c r="C6" s="1">
-        <v>189000</v>
+        <v>98724.845995893222</v>
       </c>
       <c r="D6" s="1">
-        <v>98724.845995893222</v>
-      </c>
-      <c r="E6" s="1">
         <v>134857.14285714287</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>43</v>
+      <c r="B7" s="1">
+        <v>100669.06474820143</v>
       </c>
       <c r="C7" s="1">
-        <v>100669.06474820143</v>
+        <v>44450.428396572825</v>
       </c>
       <c r="D7" s="1">
-        <v>44450.428396572825</v>
-      </c>
-      <c r="E7" s="1">
         <v>58723.287671232873</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>44</v>
+      <c r="B8" s="1">
+        <v>127816.59388646288</v>
       </c>
       <c r="C8" s="1">
-        <v>127816.59388646288</v>
+        <v>62619.589977220952</v>
       </c>
       <c r="D8" s="1">
-        <v>62619.589977220952</v>
-      </c>
-      <c r="E8" s="1">
         <v>84970.059880239511</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>45</v>
+      <c r="B9" s="1">
+        <v>95163.461538461532</v>
       </c>
       <c r="C9" s="1">
-        <v>95163.461538461532</v>
+        <v>60238.095238095244</v>
       </c>
       <c r="D9" s="1">
-        <v>60238.095238095244</v>
-      </c>
-      <c r="E9" s="1">
         <v>76030.434782608689</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>46</v>
+      <c r="B10" s="1">
+        <v>251567.42556917688</v>
       </c>
       <c r="C10" s="1">
-        <v>251567.42556917688</v>
+        <v>102682.89211500142</v>
       </c>
       <c r="D10" s="1">
-        <v>102682.89211500142</v>
-      </c>
-      <c r="E10" s="1">
         <v>151484.88327592803</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>47</v>
+      <c r="B11" s="1">
+        <v>56915.117719950431</v>
       </c>
       <c r="C11" s="1">
-        <v>56915.117719950431</v>
+        <v>16145.912187736563</v>
       </c>
       <c r="D11" s="1">
-        <v>16145.912187736563</v>
-      </c>
-      <c r="E11" s="1">
         <v>25685.126123514063</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>48</v>
+      <c r="B12" s="1">
+        <v>134859.15492957746</v>
       </c>
       <c r="C12" s="1">
-        <v>134859.15492957746</v>
+        <v>100782.62634463163</v>
       </c>
       <c r="D12" s="1">
-        <v>100782.62634463163</v>
-      </c>
-      <c r="E12" s="1">
         <v>113242.6934466332</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>49</v>
+      <c r="B13" s="1">
+        <v>119983.05084745763</v>
       </c>
       <c r="C13" s="1">
-        <v>119983.05084745763</v>
+        <v>46355.932203389835</v>
       </c>
       <c r="D13" s="1">
-        <v>46355.932203389835</v>
-      </c>
-      <c r="E13" s="1">
         <v>70898.305084745763</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
-        <v>50</v>
+      <c r="B14" s="1">
+        <v>188964.1791044776</v>
       </c>
       <c r="C14" s="1">
-        <v>188964.1791044776</v>
+        <v>95189.296771340116</v>
       </c>
       <c r="D14" s="1">
-        <v>95189.296771340116</v>
-      </c>
-      <c r="E14" s="1">
         <v>135096.03658536586</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>74</v>
+      <c r="B15" s="1">
+        <v>147111.1903064861</v>
       </c>
       <c r="C15" s="1">
-        <v>147111.1903064861</v>
+        <v>94597.609561752994</v>
       </c>
       <c r="D15" s="1">
-        <v>94597.609561752994</v>
-      </c>
-      <c r="E15" s="1">
         <v>119924.71639738741</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="B16" s="1">
+        <v>124857.14285714286</v>
       </c>
       <c r="C16" s="1">
-        <v>124857.14285714286</v>
+        <v>83327.044025157229</v>
       </c>
       <c r="D16" s="1">
-        <v>83327.044025157229</v>
-      </c>
-      <c r="E16" s="1">
         <v>102772.57525083613</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
-        <v>51</v>
+      <c r="B17" s="1">
+        <v>73271.983640081802</v>
       </c>
       <c r="C17" s="1">
-        <v>73271.983640081802</v>
+        <v>50605.194805194806</v>
       </c>
       <c r="D17" s="1">
-        <v>50605.194805194806</v>
-      </c>
-      <c r="E17" s="1">
         <v>57347.323600973235</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
-        <v>52</v>
+      <c r="B18" s="1">
+        <v>125357.54189944135</v>
       </c>
       <c r="C18" s="1">
-        <v>125357.54189944135</v>
+        <v>42347.24540901502</v>
       </c>
       <c r="D18" s="1">
-        <v>42347.24540901502</v>
-      </c>
-      <c r="E18" s="1">
         <v>61446.015424164521</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
-        <v>53</v>
+      <c r="B19" s="1">
+        <v>152828.79377431906</v>
       </c>
       <c r="C19" s="1">
-        <v>152828.79377431906</v>
+        <v>115257.51072961373</v>
       </c>
       <c r="D19" s="1">
-        <v>115257.51072961373</v>
-      </c>
-      <c r="E19" s="1">
         <v>134963.26530612246</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
-        <v>54</v>
+      <c r="B20" s="1">
+        <v>316661.57760814246</v>
       </c>
       <c r="C20" s="1">
-        <v>316661.57760814246</v>
+        <v>149023.40425531915</v>
       </c>
       <c r="D20" s="1">
-        <v>149023.40425531915</v>
-      </c>
-      <c r="E20" s="1">
         <v>225363.84704519119</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
-        <v>55</v>
+      <c r="B21" s="1">
+        <v>69452.054794520547</v>
       </c>
       <c r="C21" s="1">
-        <v>69452.054794520547</v>
+        <v>31222.627737226278</v>
       </c>
       <c r="D21" s="1">
-        <v>31222.627737226278</v>
-      </c>
-      <c r="E21" s="1">
         <v>39265.129682997118</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B22" t="s">
-        <v>56</v>
+      <c r="B22" s="1">
+        <v>125745.09803921569</v>
       </c>
       <c r="C22" s="1">
-        <v>125745.09803921569</v>
+        <v>41917.098445595853</v>
       </c>
       <c r="D22" s="1">
-        <v>41917.098445595853</v>
-      </c>
-      <c r="E22" s="1">
         <v>59438.524590163935</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
-        <v>57</v>
+      <c r="B23" s="1">
+        <v>171593.3014354067</v>
       </c>
       <c r="C23" s="1">
-        <v>171593.3014354067</v>
+        <v>132778.2656421515</v>
       </c>
       <c r="D23" s="1">
-        <v>132778.2656421515</v>
-      </c>
-      <c r="E23" s="1">
         <v>140021.42857142858</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B24" t="s">
-        <v>58</v>
+      <c r="B24" s="1">
+        <v>103765.95744680852</v>
       </c>
       <c r="C24" s="1">
-        <v>103765.95744680852</v>
+        <v>53389.380530973453</v>
       </c>
       <c r="D24" s="1">
-        <v>53389.380530973453</v>
-      </c>
-      <c r="E24" s="1">
         <v>68187.5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B25" t="s">
-        <v>75</v>
+      <c r="B25" s="1">
+        <v>66000</v>
       </c>
       <c r="C25" s="1">
-        <v>66000</v>
+        <v>28366.515837104071</v>
       </c>
       <c r="D25" s="1">
-        <v>28366.515837104071</v>
-      </c>
-      <c r="E25" s="1">
         <v>36507.092198581558</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B26" t="s">
-        <v>59</v>
+      <c r="B26" s="1">
+        <v>26953.846153846152</v>
       </c>
       <c r="C26" s="1">
-        <v>26953.846153846152</v>
+        <v>13468.75</v>
       </c>
       <c r="D26" s="1">
-        <v>13468.75</v>
-      </c>
-      <c r="E26" s="1">
         <v>17364.444444444445</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
-      <c r="B27" t="s">
-        <v>60</v>
+      <c r="B27" s="1">
+        <v>339375.54585152841</v>
       </c>
       <c r="C27" s="1">
-        <v>339375.54585152841</v>
+        <v>182829.88505747129</v>
       </c>
       <c r="D27" s="1">
-        <v>182829.88505747129</v>
-      </c>
-      <c r="E27" s="1">
         <v>236819.27710843374</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B28" t="s">
-        <v>61</v>
+      <c r="B28" s="1">
+        <v>172697.01853344077</v>
       </c>
       <c r="C28" s="1">
-        <v>172697.01853344077</v>
+        <v>80436.225371586581</v>
       </c>
       <c r="D28" s="1">
-        <v>80436.225371586581</v>
-      </c>
-      <c r="E28" s="1">
         <v>108132.31736816642</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
-      <c r="B29" t="s">
-        <v>62</v>
+      <c r="B29" s="1">
+        <v>274070</v>
       </c>
       <c r="C29" s="1">
-        <v>274070</v>
+        <v>90555.555555555562</v>
       </c>
       <c r="D29" s="1">
-        <v>90555.555555555562</v>
-      </c>
-      <c r="E29" s="1">
         <v>144058.30903790088</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="B30" t="s">
-        <v>63</v>
+      <c r="B30" s="1">
+        <v>169465.90909090909</v>
       </c>
       <c r="C30" s="1">
-        <v>169465.90909090909</v>
+        <v>118675.92592592593</v>
       </c>
       <c r="D30" s="1">
-        <v>118675.92592592593</v>
-      </c>
-      <c r="E30" s="1">
         <v>133378.28947368421</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
-      <c r="B31" t="s">
-        <v>64</v>
+      <c r="B31" s="1">
+        <v>77367.088607594938</v>
       </c>
       <c r="C31" s="1">
-        <v>77367.088607594938</v>
+        <v>42270.408163265311</v>
       </c>
       <c r="D31" s="1">
-        <v>42270.408163265311</v>
-      </c>
-      <c r="E31" s="1">
         <v>52352.727272727272</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
-      <c r="B32" t="s">
-        <v>65</v>
+      <c r="B32" s="1">
+        <v>114025.64102564102</v>
       </c>
       <c r="C32" s="1">
-        <v>114025.64102564102</v>
+        <v>44840.891621829367</v>
       </c>
       <c r="D32" s="1">
-        <v>44840.891621829367</v>
-      </c>
-      <c r="E32" s="1">
         <v>66300.636267232228</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
-      <c r="B33" t="s">
-        <v>66</v>
+      <c r="B33" s="1">
+        <v>120702.21327967806</v>
       </c>
       <c r="C33" s="1">
-        <v>120702.21327967806</v>
+        <v>78693.059628543488</v>
       </c>
       <c r="D33" s="1">
-        <v>78693.059628543488</v>
-      </c>
-      <c r="E33" s="1">
         <v>92428.947368421053</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="B34" t="s">
-        <v>67</v>
+      <c r="B34" s="1">
+        <v>24411.764705882353</v>
       </c>
       <c r="C34" s="1">
-        <v>24411.764705882353</v>
+        <v>13663.608562691132</v>
       </c>
       <c r="D34" s="1">
-        <v>13663.608562691132</v>
-      </c>
-      <c r="E34" s="1">
         <v>15113.756613756614</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" t="s">
-        <v>72</v>
+        <v>37</v>
+      </c>
+      <c r="B35" s="1">
+        <v>205340.5172413793</v>
       </c>
       <c r="C35" s="1">
-        <v>205340.5172413793</v>
+        <v>143303.35097001764</v>
       </c>
       <c r="D35" s="1">
-        <v>143303.35097001764</v>
-      </c>
-      <c r="E35" s="1">
         <v>161316.64580725908</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>29</v>
       </c>
-      <c r="B36" t="s">
-        <v>68</v>
+      <c r="B36" s="1">
+        <v>235688.7159533074</v>
       </c>
       <c r="C36" s="1">
-        <v>235688.7159533074</v>
+        <v>169382.06627680312</v>
       </c>
       <c r="D36" s="1">
-        <v>169382.06627680312</v>
-      </c>
-      <c r="E36" s="1">
         <v>182664.06858924395</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>30</v>
       </c>
-      <c r="B37" t="s">
-        <v>69</v>
+      <c r="B37" s="1">
+        <v>112614.4578313253</v>
       </c>
       <c r="C37" s="1">
-        <v>112614.4578313253</v>
+        <v>81471.42857142858</v>
       </c>
       <c r="D37" s="1">
-        <v>81471.42857142858</v>
-      </c>
-      <c r="E37" s="1">
         <v>93062.78026905829</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>31</v>
       </c>
-      <c r="B38" t="s">
-        <v>70</v>
+      <c r="B38" s="1">
+        <v>65392.739273927393</v>
       </c>
       <c r="C38" s="1">
-        <v>65392.739273927393</v>
+        <v>48350.77519379845</v>
       </c>
       <c r="D38" s="1">
-        <v>48350.77519379845</v>
-      </c>
-      <c r="E38" s="1">
         <v>54655.67765567766</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>32</v>
       </c>
-      <c r="B39" t="s">
-        <v>71</v>
+      <c r="B39" s="1">
+        <v>30960.216998191681</v>
       </c>
       <c r="C39" s="1">
-        <v>30960.216998191681</v>
+        <v>23221.42064372919</v>
       </c>
       <c r="D39" s="1">
-        <v>23221.42064372919</v>
-      </c>
-      <c r="E39" s="1">
         <v>25038.64118895966</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" t="s">
-        <v>87</v>
+        <v>48</v>
+      </c>
+      <c r="B40" s="1">
+        <v>150662.18622551553</v>
       </c>
       <c r="C40" s="1">
-        <v>150662.18622551553</v>
+        <v>74359.694558658623</v>
       </c>
       <c r="D40" s="1">
-        <v>74359.694558658623</v>
-      </c>
-      <c r="E40" s="1">
         <v>98571.824362502972</v>
       </c>
     </row>
@@ -2535,15 +2294,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="841a37d2-6ac6-4cb8-8211-c8824e7b4dcd">
@@ -2552,6 +2302,15 @@
     <TaxCatchAll xmlns="c78a888a-83d8-49bb-8890-6eb97e8a3c0e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2574,14 +2333,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B31F663-6144-4024-83F4-0C35A9D0D635}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3ADF35-F119-4BE6-85A8-2E5C6C3A1AE7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2596,4 +2347,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B31F663-6144-4024-83F4-0C35A9D0D635}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>